<commit_message>
-validation scripts -ext forms / ext store - new module for OConnor, checked in on behalf of Paul Hines.
SVN r15704 |2011-03-01 18:32:36 +0000
</commit_message>
<xml_diff>
--- a/ehr/tools/PrePopulateData/Task Data.xlsx
+++ b/ehr/tools/PrePopulateData/Task Data.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4885" uniqueCount="1652">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4953" uniqueCount="1661">
   <si>
     <t>tasktype</t>
   </si>
@@ -4978,6 +4978,33 @@
   </si>
   <si>
     <t>@e-00040</t>
+  </si>
+  <si>
+    <t>Blood Chemistry</t>
+  </si>
+  <si>
+    <t>Virology Runs</t>
+  </si>
+  <si>
+    <t>Hematology Runs</t>
+  </si>
+  <si>
+    <t>Hematology Results</t>
+  </si>
+  <si>
+    <t>Immunology Runs</t>
+  </si>
+  <si>
+    <t>Immunology Results</t>
+  </si>
+  <si>
+    <t>Blood Chemistry Runs</t>
+  </si>
+  <si>
+    <t>Blood Chemistry Results</t>
+  </si>
+  <si>
+    <t>Task,Assay</t>
   </si>
 </sst>
 </file>
@@ -5338,10 +5365,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E11"/>
+      <selection activeCell="E12" sqref="E12:E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5384,7 +5411,7 @@
         <v>28</v>
       </c>
       <c r="E3" t="str">
-        <f t="shared" ref="E3:E11" si="0">CONCATENATE("['",A3,"', '",B3,"', '",C3,"', '",D3,"'],")</f>
+        <f t="shared" ref="E3:E15" si="0">CONCATENATE("['",A3,"', '",B3,"', '",C3,"', '",D3,"'],")</f>
         <v>['Irregular Observations', 'Task', '', ''],</v>
       </c>
     </row>
@@ -5480,8 +5507,56 @@
         <v>433</v>
       </c>
       <c r="E11" t="str">
+        <f>CONCATENATE("['",A11,"', '",B11,"', '",C11,"', '",D11,"'],")</f>
+        <v>['Housing Request', 'Request', '', ''],</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" t="s">
+        <v>80</v>
+      </c>
+      <c r="B12" t="s">
+        <v>28</v>
+      </c>
+      <c r="E12" t="str">
         <f t="shared" si="0"/>
-        <v>['Housing Request', 'Request', '', ''],</v>
+        <v>['Virology', 'Task', '', ''],</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" t="s">
+        <v>62</v>
+      </c>
+      <c r="B13" t="s">
+        <v>28</v>
+      </c>
+      <c r="E13" t="str">
+        <f t="shared" si="0"/>
+        <v>['Hematology', 'Task', '', ''],</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" t="s">
+        <v>130</v>
+      </c>
+      <c r="B14" t="s">
+        <v>28</v>
+      </c>
+      <c r="E14" t="str">
+        <f t="shared" si="0"/>
+        <v>['Immunology', 'Task', '', ''],</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" t="s">
+        <v>1652</v>
+      </c>
+      <c r="B15" t="s">
+        <v>28</v>
+      </c>
+      <c r="E15" t="str">
+        <f t="shared" si="0"/>
+        <v>['Blood Chemistry', 'Task', '', ''],</v>
       </c>
     </row>
   </sheetData>
@@ -5492,11 +5567,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L47"/>
+  <dimension ref="A1:L59"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B32" sqref="B32"/>
+      <pane ySplit="1" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C49" sqref="C49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5590,7 +5665,7 @@
         <v>2</v>
       </c>
       <c r="L3" t="str">
-        <f t="shared" ref="L3:L47" si="0">CONCATENATE("['",A3,"' ,'",B3,"' ,'",C3,"' ,'",D3,"' ,'",E3,"', '",F3,"', '",G3,"', '",H3,"', '",I3,"', '",J3,"', '",K3,"'],")</f>
+        <f t="shared" ref="L3:L59" si="0">CONCATENATE("['",A3,"' ,'",B3,"' ,'",C3,"' ,'",D3,"' ,'",E3,"', '",F3,"', '",G3,"', '",H3,"', '",I3,"', '",J3,"', '",K3,"'],")</f>
         <v>['Physical Exam' ,'formSections' ,'ehr-abstractpanel' ,'2' ,'', '', '', '', '', '', ''],</v>
       </c>
     </row>
@@ -6750,6 +6825,291 @@
       <c r="L47" t="str">
         <f t="shared" si="0"/>
         <v>['Housing Request' ,'formSections' ,'ehr-gridformpanel' ,'2' ,'Housing', 'study', '', 'Task,Request', '', '', ''],</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12">
+      <c r="A48" t="s">
+        <v>80</v>
+      </c>
+      <c r="B48" t="s">
+        <v>42</v>
+      </c>
+      <c r="C48" t="s">
+        <v>9</v>
+      </c>
+      <c r="D48">
+        <v>1</v>
+      </c>
+      <c r="L48" t="str">
+        <f t="shared" si="0"/>
+        <v>['Virology' ,'formSections' ,'ehr-abstractpanel' ,'1' ,'', '', '', '', '', '', ''],</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12">
+      <c r="A49" t="s">
+        <v>80</v>
+      </c>
+      <c r="B49" t="s">
+        <v>42</v>
+      </c>
+      <c r="C49" t="s">
+        <v>13</v>
+      </c>
+      <c r="D49">
+        <v>2</v>
+      </c>
+      <c r="E49" t="s">
+        <v>1653</v>
+      </c>
+      <c r="F49" t="s">
+        <v>12</v>
+      </c>
+      <c r="H49" t="s">
+        <v>1660</v>
+      </c>
+      <c r="L49" t="str">
+        <f t="shared" si="0"/>
+        <v>['Virology' ,'formSections' ,'ehr-formpanel' ,'2' ,'Virology Runs', 'study', '', 'Task,Assay', '', '', ''],</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12">
+      <c r="A50" t="s">
+        <v>80</v>
+      </c>
+      <c r="B50" t="s">
+        <v>42</v>
+      </c>
+      <c r="C50" t="s">
+        <v>10</v>
+      </c>
+      <c r="E50" t="s">
+        <v>139</v>
+      </c>
+      <c r="F50" t="s">
+        <v>12</v>
+      </c>
+      <c r="H50" t="s">
+        <v>1660</v>
+      </c>
+      <c r="L50" t="str">
+        <f t="shared" si="0"/>
+        <v>['Virology' ,'formSections' ,'ehr-gridformpanel' ,'' ,'Virology Results', 'study', '', 'Task,Assay', '', '', ''],</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12">
+      <c r="A51" t="s">
+        <v>62</v>
+      </c>
+      <c r="B51" t="s">
+        <v>42</v>
+      </c>
+      <c r="C51" t="s">
+        <v>9</v>
+      </c>
+      <c r="D51">
+        <v>1</v>
+      </c>
+      <c r="L51" t="str">
+        <f t="shared" si="0"/>
+        <v>['Hematology' ,'formSections' ,'ehr-abstractpanel' ,'1' ,'', '', '', '', '', '', ''],</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12">
+      <c r="A52" t="s">
+        <v>62</v>
+      </c>
+      <c r="B52" t="s">
+        <v>42</v>
+      </c>
+      <c r="C52" t="s">
+        <v>13</v>
+      </c>
+      <c r="D52">
+        <v>2</v>
+      </c>
+      <c r="E52" t="s">
+        <v>1654</v>
+      </c>
+      <c r="F52" t="s">
+        <v>12</v>
+      </c>
+      <c r="H52" t="s">
+        <v>1660</v>
+      </c>
+      <c r="L52" t="str">
+        <f t="shared" si="0"/>
+        <v>['Hematology' ,'formSections' ,'ehr-formpanel' ,'2' ,'Hematology Runs', 'study', '', 'Task,Assay', '', '', ''],</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12">
+      <c r="A53" t="s">
+        <v>62</v>
+      </c>
+      <c r="B53" t="s">
+        <v>42</v>
+      </c>
+      <c r="C53" t="s">
+        <v>10</v>
+      </c>
+      <c r="D53">
+        <v>3</v>
+      </c>
+      <c r="E53" t="s">
+        <v>1655</v>
+      </c>
+      <c r="F53" t="s">
+        <v>12</v>
+      </c>
+      <c r="H53" t="s">
+        <v>1660</v>
+      </c>
+      <c r="L53" t="str">
+        <f t="shared" si="0"/>
+        <v>['Hematology' ,'formSections' ,'ehr-gridformpanel' ,'3' ,'Hematology Results', 'study', '', 'Task,Assay', '', '', ''],</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12">
+      <c r="A54" t="s">
+        <v>130</v>
+      </c>
+      <c r="B54" t="s">
+        <v>42</v>
+      </c>
+      <c r="C54" t="s">
+        <v>9</v>
+      </c>
+      <c r="D54">
+        <v>1</v>
+      </c>
+      <c r="L54" t="str">
+        <f t="shared" si="0"/>
+        <v>['Immunology' ,'formSections' ,'ehr-abstractpanel' ,'1' ,'', '', '', '', '', '', ''],</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12">
+      <c r="A55" t="s">
+        <v>130</v>
+      </c>
+      <c r="B55" t="s">
+        <v>42</v>
+      </c>
+      <c r="C55" t="s">
+        <v>13</v>
+      </c>
+      <c r="D55">
+        <v>2</v>
+      </c>
+      <c r="E55" t="s">
+        <v>1656</v>
+      </c>
+      <c r="F55" t="s">
+        <v>12</v>
+      </c>
+      <c r="H55" t="s">
+        <v>1660</v>
+      </c>
+      <c r="L55" t="str">
+        <f t="shared" si="0"/>
+        <v>['Immunology' ,'formSections' ,'ehr-formpanel' ,'2' ,'Immunology Runs', 'study', '', 'Task,Assay', '', '', ''],</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12">
+      <c r="A56" t="s">
+        <v>130</v>
+      </c>
+      <c r="B56" t="s">
+        <v>42</v>
+      </c>
+      <c r="C56" t="s">
+        <v>10</v>
+      </c>
+      <c r="D56">
+        <v>3</v>
+      </c>
+      <c r="E56" t="s">
+        <v>1657</v>
+      </c>
+      <c r="F56" t="s">
+        <v>12</v>
+      </c>
+      <c r="H56" t="s">
+        <v>1660</v>
+      </c>
+      <c r="L56" t="str">
+        <f t="shared" si="0"/>
+        <v>['Immunology' ,'formSections' ,'ehr-gridformpanel' ,'3' ,'Immunology Results', 'study', '', 'Task,Assay', '', '', ''],</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12">
+      <c r="A57" t="s">
+        <v>1652</v>
+      </c>
+      <c r="B57" t="s">
+        <v>42</v>
+      </c>
+      <c r="C57" t="s">
+        <v>9</v>
+      </c>
+      <c r="D57">
+        <v>1</v>
+      </c>
+      <c r="L57" t="str">
+        <f t="shared" si="0"/>
+        <v>['Blood Chemistry' ,'formSections' ,'ehr-abstractpanel' ,'1' ,'', '', '', '', '', '', ''],</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12">
+      <c r="A58" t="s">
+        <v>1652</v>
+      </c>
+      <c r="B58" t="s">
+        <v>42</v>
+      </c>
+      <c r="C58" t="s">
+        <v>13</v>
+      </c>
+      <c r="D58">
+        <v>2</v>
+      </c>
+      <c r="E58" t="s">
+        <v>1658</v>
+      </c>
+      <c r="F58" t="s">
+        <v>12</v>
+      </c>
+      <c r="H58" t="s">
+        <v>1660</v>
+      </c>
+      <c r="L58" t="str">
+        <f t="shared" si="0"/>
+        <v>['Blood Chemistry' ,'formSections' ,'ehr-formpanel' ,'2' ,'Blood Chemistry Runs', 'study', '', 'Task,Assay', '', '', ''],</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12">
+      <c r="A59" t="s">
+        <v>1652</v>
+      </c>
+      <c r="B59" t="s">
+        <v>42</v>
+      </c>
+      <c r="C59" t="s">
+        <v>10</v>
+      </c>
+      <c r="D59">
+        <v>3</v>
+      </c>
+      <c r="E59" t="s">
+        <v>1659</v>
+      </c>
+      <c r="F59" t="s">
+        <v>12</v>
+      </c>
+      <c r="H59" t="s">
+        <v>1660</v>
+      </c>
+      <c r="L59" t="str">
+        <f t="shared" si="0"/>
+        <v>['Blood Chemistry' ,'formSections' ,'ehr-gridformpanel' ,'3' ,'Blood Chemistry Results', 'study', '', 'Task,Assay', '', '', ''],</v>
       </c>
     </row>
   </sheetData>

</xml_diff>